<commit_message>
Debut de Reconnaissance Vocale
C'est pas encore parfait mais c'est un début avec un concept de corrélation entre deux FFT. Il faut que je fasse des moyennes de FFT pour que la valeur soit plus stable et que ça ne réagisse que à ça.
</commit_message>
<xml_diff>
--- a/Projet/Calcul dB.xlsx
+++ b/Projet/Calcul dB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85e7673ddcb14ddb/Documents/PlatformIO/Projects/Reconnaissance-Vocale/Projet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5547991-004F-4A95-8497-4855271336BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{C5547991-004F-4A95-8497-4855271336BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB1B9D13-6E61-4020-B5A4-634165AFBF4C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{922D7660-369A-4C6C-BD8E-AD8A21C21B19}"/>
   </bookViews>
@@ -35,12 +35,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>V</t>
   </si>
   <si>
     <t>dB</t>
+  </si>
+  <si>
+    <t>Valeurs 1</t>
+  </si>
+  <si>
+    <t>Valeurs 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somme 1 et 2 </t>
+  </si>
+  <si>
+    <t>1 carre</t>
+  </si>
+  <si>
+    <t>2 carre</t>
+  </si>
+  <si>
+    <t>Somme :</t>
+  </si>
+  <si>
+    <t>Correlation normative :</t>
+  </si>
+  <si>
+    <t>Valeurs 3</t>
   </si>
 </sst>
 </file>
@@ -468,7 +492,740 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$K$2:$K$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0">
+                  <c:v>7088.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4620.0200000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1432.46</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>724.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>563.69000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>201.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.66</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.43</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50.05</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>176.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>218.14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>178.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>94.23</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>66.58</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>38.130000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>34.909999999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>56.52</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>80.959999999999994</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>86.87</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>153.97999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>154.59</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>161.69</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>45.31</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>50.49</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>61.33</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>50.48</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>59.06</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>92.04</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>31.73</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>114.24</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>137.84</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>126.26</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>38.44</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>126.26</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>137.84</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>114.24</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>31.73</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>92.04</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>59.06</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>50.48</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>61.33</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>50.49</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45.31</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>161.69</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>154.59</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>153.97999999999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>86.87</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>80.959999999999994</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>56.52</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>34.909999999999997</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>38.130000000000003</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>66.58</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>94.23</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>178.7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>218.14</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>176.8</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>50.05</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>40.43</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>18.66</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>201.53</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>563.69000000000005</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>724.93</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1432.46</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4620.0200000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C7D9-4FEB-BB9E-52BA98B08C96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$L$2:$L$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0">
+                  <c:v>8365.16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5316</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1693.71</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>745.69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>405.17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.78</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>198.53</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>178.57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>107.13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90.98</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.760000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>82.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>148.09</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>131.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24.73</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>65.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>69.28</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>76.25</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40.770000000000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40.92</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>93.04</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>104.96</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>71.72</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>56.42</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18.350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>38.6</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>67.33</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>19.309999999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>62.62</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>48.79</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>71.41</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>48.79</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>62.62</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>19.309999999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>67.33</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>18.350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>56.42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>71.72</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>104.96</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>93.04</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>40.92</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>40.770000000000003</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>76.25</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>69.28</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>65.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>24.73</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>131.6</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>148.09</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>82.8</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>33.1</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>19.760000000000002</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>90.98</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>107.13</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>178.57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>28.02</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>198.53</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>99.78</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>405.17</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>745.69</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1693.71</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5316</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C7D9-4FEB-BB9E-52BA98B08C96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1018560687"/>
+        <c:axId val="1018567343"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1018560687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1018567343"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1018567343"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1018560687"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1005,6 +1762,509 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1057,6 +2317,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>283882</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>567765</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>11953</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A256E1BE-3D9C-C025-78AA-4CEEA064E80B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1362,68 +2658,1581 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947A4A9D-30F0-4C7B-B54A-FCFE21B31228}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M73" sqref="M73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>200</v>
       </c>
       <c r="B2">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J2">
+        <v>5178.2</v>
+      </c>
+      <c r="K2">
+        <v>7088.52</v>
+      </c>
+      <c r="L2">
+        <v>8365.16</v>
+      </c>
+      <c r="M2">
+        <f>K2+L2</f>
+        <v>15453.68</v>
+      </c>
+      <c r="N2">
+        <f>K2^2</f>
+        <v>50247115.790400006</v>
+      </c>
+      <c r="O2">
+        <f>L2^2</f>
+        <v>69975901.825599998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>320</v>
       </c>
       <c r="B3">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <v>1334.54</v>
+      </c>
+      <c r="K3">
+        <v>4620.0200000000004</v>
+      </c>
+      <c r="L3">
+        <v>5316</v>
+      </c>
+      <c r="M3">
+        <f>K3+L3</f>
+        <v>9936.02</v>
+      </c>
+      <c r="N3">
+        <f>K3^2</f>
+        <v>21344584.800400004</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O65" si="0">L3^2</f>
+        <v>28259856</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>450</v>
       </c>
       <c r="B4">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <v>1240.48</v>
+      </c>
+      <c r="K4">
+        <v>1432.46</v>
+      </c>
+      <c r="L4">
+        <v>1693.71</v>
+      </c>
+      <c r="M4">
+        <f>K4+L4</f>
+        <v>3126.17</v>
+      </c>
+      <c r="N4">
+        <f>K4^2</f>
+        <v>2051941.6516000002</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>2868653.5641000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>600</v>
       </c>
       <c r="B5">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <v>875.73</v>
+      </c>
+      <c r="K5">
+        <v>724.93</v>
+      </c>
+      <c r="L5">
+        <v>745.69</v>
+      </c>
+      <c r="M5">
+        <f>K5+L5</f>
+        <v>1470.62</v>
+      </c>
+      <c r="N5">
+        <f>K5^2</f>
+        <v>525523.50489999994</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>556053.57610000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>800</v>
       </c>
       <c r="B6">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J6">
+        <v>358.79</v>
+      </c>
+      <c r="K6">
+        <v>563.69000000000005</v>
+      </c>
+      <c r="L6">
+        <v>405.17</v>
+      </c>
+      <c r="M6">
+        <f>K6+L6</f>
+        <v>968.86000000000013</v>
+      </c>
+      <c r="N6">
+        <f>K6^2</f>
+        <v>317746.41610000009</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>164162.72890000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1023</v>
       </c>
       <c r="B7">
         <v>90</v>
+      </c>
+      <c r="J7">
+        <v>123.97</v>
+      </c>
+      <c r="K7">
+        <v>201.53</v>
+      </c>
+      <c r="L7">
+        <v>99.78</v>
+      </c>
+      <c r="M7">
+        <f>K7+L7</f>
+        <v>301.31</v>
+      </c>
+      <c r="N7">
+        <f>K7^2</f>
+        <v>40614.340900000003</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>9956.0483999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J8">
+        <v>201.42</v>
+      </c>
+      <c r="K8">
+        <v>18.66</v>
+      </c>
+      <c r="L8">
+        <v>198.53</v>
+      </c>
+      <c r="M8">
+        <f>K8+L8</f>
+        <v>217.19</v>
+      </c>
+      <c r="N8">
+        <f>K8^2</f>
+        <v>348.19560000000001</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>39414.160900000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J9">
+        <v>139.15</v>
+      </c>
+      <c r="K9">
+        <v>40.43</v>
+      </c>
+      <c r="L9">
+        <v>28.02</v>
+      </c>
+      <c r="M9">
+        <f>K9+L9</f>
+        <v>68.45</v>
+      </c>
+      <c r="N9">
+        <f>K9^2</f>
+        <v>1634.5849000000001</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>785.12040000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J10">
+        <v>138.85</v>
+      </c>
+      <c r="K10">
+        <v>50.05</v>
+      </c>
+      <c r="L10">
+        <v>178.57</v>
+      </c>
+      <c r="M10">
+        <f>K10+L10</f>
+        <v>228.62</v>
+      </c>
+      <c r="N10">
+        <f>K10^2</f>
+        <v>2505.0024999999996</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>31887.244899999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J11">
+        <v>266.58999999999997</v>
+      </c>
+      <c r="K11">
+        <v>176.8</v>
+      </c>
+      <c r="L11">
+        <v>107.13</v>
+      </c>
+      <c r="M11">
+        <f>K11+L11</f>
+        <v>283.93</v>
+      </c>
+      <c r="N11">
+        <f>K11^2</f>
+        <v>31258.240000000005</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>11476.836899999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J12">
+        <v>239.16</v>
+      </c>
+      <c r="K12">
+        <v>218.14</v>
+      </c>
+      <c r="L12">
+        <v>90.98</v>
+      </c>
+      <c r="M12">
+        <f>K12+L12</f>
+        <v>309.12</v>
+      </c>
+      <c r="N12">
+        <f>K12^2</f>
+        <v>47585.059599999993</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>8277.3604000000014</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J13">
+        <v>81.290000000000006</v>
+      </c>
+      <c r="K13">
+        <v>178.7</v>
+      </c>
+      <c r="L13">
+        <v>19.760000000000002</v>
+      </c>
+      <c r="M13">
+        <f>K13+L13</f>
+        <v>198.45999999999998</v>
+      </c>
+      <c r="N13">
+        <f>K13^2</f>
+        <v>31933.689999999995</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>390.45760000000007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J14">
+        <v>87.91</v>
+      </c>
+      <c r="K14">
+        <v>94.23</v>
+      </c>
+      <c r="L14">
+        <v>33.1</v>
+      </c>
+      <c r="M14">
+        <f>K14+L14</f>
+        <v>127.33000000000001</v>
+      </c>
+      <c r="N14">
+        <f>K14^2</f>
+        <v>8879.2929000000004</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>1095.6100000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J15">
+        <v>95.84</v>
+      </c>
+      <c r="K15">
+        <v>66.58</v>
+      </c>
+      <c r="L15">
+        <v>82.8</v>
+      </c>
+      <c r="M15">
+        <f>K15+L15</f>
+        <v>149.38</v>
+      </c>
+      <c r="N15">
+        <f>K15^2</f>
+        <v>4432.8963999999996</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>6855.8399999999992</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J16">
+        <v>109.27</v>
+      </c>
+      <c r="K16">
+        <v>38.130000000000003</v>
+      </c>
+      <c r="L16">
+        <v>148.09</v>
+      </c>
+      <c r="M16">
+        <f>K16+L16</f>
+        <v>186.22</v>
+      </c>
+      <c r="N16">
+        <f>K16^2</f>
+        <v>1453.8969000000002</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>21930.648100000002</v>
+      </c>
+    </row>
+    <row r="17" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J17">
+        <v>256.73</v>
+      </c>
+      <c r="K17">
+        <v>34.909999999999997</v>
+      </c>
+      <c r="L17">
+        <v>131.6</v>
+      </c>
+      <c r="M17">
+        <f>K17+L17</f>
+        <v>166.51</v>
+      </c>
+      <c r="N17">
+        <f>K17^2</f>
+        <v>1218.7080999999998</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>17318.559999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J18">
+        <v>149.55000000000001</v>
+      </c>
+      <c r="K18">
+        <v>56.52</v>
+      </c>
+      <c r="L18">
+        <v>24.73</v>
+      </c>
+      <c r="M18">
+        <f>K18+L18</f>
+        <v>81.25</v>
+      </c>
+      <c r="N18">
+        <f>K18^2</f>
+        <v>3194.5104000000006</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="0"/>
+        <v>611.5729</v>
+      </c>
+    </row>
+    <row r="19" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J19">
+        <v>59.9</v>
+      </c>
+      <c r="K19">
+        <v>80.959999999999994</v>
+      </c>
+      <c r="L19">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="M19">
+        <f>K19+L19</f>
+        <v>146.56</v>
+      </c>
+      <c r="N19">
+        <f>K19^2</f>
+        <v>6554.5215999999991</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="0"/>
+        <v>4303.3599999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J20">
+        <v>49.17</v>
+      </c>
+      <c r="K20">
+        <v>86.87</v>
+      </c>
+      <c r="L20">
+        <v>69.28</v>
+      </c>
+      <c r="M20">
+        <f>K20+L20</f>
+        <v>156.15</v>
+      </c>
+      <c r="N20">
+        <f>K20^2</f>
+        <v>7546.3969000000006</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="0"/>
+        <v>4799.7183999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J21">
+        <v>47.03</v>
+      </c>
+      <c r="K21">
+        <v>153.97999999999999</v>
+      </c>
+      <c r="L21">
+        <v>76.25</v>
+      </c>
+      <c r="M21">
+        <f>K21+L21</f>
+        <v>230.23</v>
+      </c>
+      <c r="N21">
+        <f>K21^2</f>
+        <v>23709.840399999997</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="0"/>
+        <v>5814.0625</v>
+      </c>
+    </row>
+    <row r="22" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J22">
+        <v>24.56</v>
+      </c>
+      <c r="K22">
+        <v>154.59</v>
+      </c>
+      <c r="L22">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="M22">
+        <f>K22+L22</f>
+        <v>195.36</v>
+      </c>
+      <c r="N22">
+        <f>K22^2</f>
+        <v>23898.0681</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="0"/>
+        <v>1662.1929000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J23">
+        <v>35.409999999999997</v>
+      </c>
+      <c r="K23">
+        <v>161.69</v>
+      </c>
+      <c r="L23">
+        <v>40.92</v>
+      </c>
+      <c r="M23">
+        <f>K23+L23</f>
+        <v>202.61</v>
+      </c>
+      <c r="N23">
+        <f>K23^2</f>
+        <v>26143.6561</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="0"/>
+        <v>1674.4464</v>
+      </c>
+    </row>
+    <row r="24" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J24">
+        <v>55.97</v>
+      </c>
+      <c r="K24">
+        <v>45.31</v>
+      </c>
+      <c r="L24">
+        <v>93.04</v>
+      </c>
+      <c r="M24">
+        <f>K24+L24</f>
+        <v>138.35000000000002</v>
+      </c>
+      <c r="N24">
+        <f>K24^2</f>
+        <v>2052.9961000000003</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="0"/>
+        <v>8656.4416000000019</v>
+      </c>
+    </row>
+    <row r="25" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J25">
+        <v>38.83</v>
+      </c>
+      <c r="K25">
+        <v>50.49</v>
+      </c>
+      <c r="L25">
+        <v>104.96</v>
+      </c>
+      <c r="M25">
+        <f>K25+L25</f>
+        <v>155.44999999999999</v>
+      </c>
+      <c r="N25">
+        <f>K25^2</f>
+        <v>2549.2401</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="0"/>
+        <v>11016.601599999998</v>
+      </c>
+    </row>
+    <row r="26" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J26">
+        <v>97.42</v>
+      </c>
+      <c r="K26">
+        <v>61.33</v>
+      </c>
+      <c r="L26">
+        <v>71.72</v>
+      </c>
+      <c r="M26">
+        <f>K26+L26</f>
+        <v>133.05000000000001</v>
+      </c>
+      <c r="N26">
+        <f>K26^2</f>
+        <v>3761.3688999999999</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="0"/>
+        <v>5143.7583999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J27">
+        <v>78.36</v>
+      </c>
+      <c r="K27">
+        <v>50.48</v>
+      </c>
+      <c r="L27">
+        <v>56.42</v>
+      </c>
+      <c r="M27">
+        <f>K27+L27</f>
+        <v>106.9</v>
+      </c>
+      <c r="N27">
+        <f>K27^2</f>
+        <v>2548.2303999999995</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="0"/>
+        <v>3183.2164000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J28">
+        <v>62.94</v>
+      </c>
+      <c r="K28">
+        <v>59.06</v>
+      </c>
+      <c r="L28">
+        <v>18.350000000000001</v>
+      </c>
+      <c r="M28">
+        <f>K28+L28</f>
+        <v>77.41</v>
+      </c>
+      <c r="N28">
+        <f>K28^2</f>
+        <v>3488.0836000000004</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="0"/>
+        <v>336.72250000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J29">
+        <v>28.98</v>
+      </c>
+      <c r="K29">
+        <v>92.04</v>
+      </c>
+      <c r="L29">
+        <v>38.6</v>
+      </c>
+      <c r="M29">
+        <f>K29+L29</f>
+        <v>130.64000000000001</v>
+      </c>
+      <c r="N29">
+        <f>K29^2</f>
+        <v>8471.361600000002</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="0"/>
+        <v>1489.96</v>
+      </c>
+    </row>
+    <row r="30" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J30">
+        <v>28.75</v>
+      </c>
+      <c r="K30">
+        <v>31.73</v>
+      </c>
+      <c r="L30">
+        <v>67.33</v>
+      </c>
+      <c r="M30">
+        <f>K30+L30</f>
+        <v>99.06</v>
+      </c>
+      <c r="N30">
+        <f>K30^2</f>
+        <v>1006.7929</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="0"/>
+        <v>4533.3288999999995</v>
+      </c>
+    </row>
+    <row r="31" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J31">
+        <v>27.86</v>
+      </c>
+      <c r="K31">
+        <v>114.24</v>
+      </c>
+      <c r="L31">
+        <v>19.309999999999999</v>
+      </c>
+      <c r="M31">
+        <f>K31+L31</f>
+        <v>133.54999999999998</v>
+      </c>
+      <c r="N31">
+        <f>K31^2</f>
+        <v>13050.777599999999</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="0"/>
+        <v>372.87609999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J32">
+        <v>28.96</v>
+      </c>
+      <c r="K32">
+        <v>137.84</v>
+      </c>
+      <c r="L32">
+        <v>62.62</v>
+      </c>
+      <c r="M32">
+        <f>K32+L32</f>
+        <v>200.46</v>
+      </c>
+      <c r="N32">
+        <f>K32^2</f>
+        <v>18999.865600000001</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="0"/>
+        <v>3921.2643999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J33">
+        <v>21.3</v>
+      </c>
+      <c r="K33">
+        <v>126.26</v>
+      </c>
+      <c r="L33">
+        <v>48.79</v>
+      </c>
+      <c r="M33">
+        <f>K33+L33</f>
+        <v>175.05</v>
+      </c>
+      <c r="N33">
+        <f>K33^2</f>
+        <v>15941.587600000001</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="0"/>
+        <v>2380.4641000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J34">
+        <v>6.8</v>
+      </c>
+      <c r="K34">
+        <v>38.44</v>
+      </c>
+      <c r="L34">
+        <v>71.41</v>
+      </c>
+      <c r="M34">
+        <f>K34+L34</f>
+        <v>109.85</v>
+      </c>
+      <c r="N34">
+        <f>K34^2</f>
+        <v>1477.6335999999999</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="0"/>
+        <v>5099.3880999999992</v>
+      </c>
+    </row>
+    <row r="35" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J35">
+        <v>21.3</v>
+      </c>
+      <c r="K35">
+        <v>126.26</v>
+      </c>
+      <c r="L35">
+        <v>48.79</v>
+      </c>
+      <c r="M35">
+        <f>K35+L35</f>
+        <v>175.05</v>
+      </c>
+      <c r="N35">
+        <f>K35^2</f>
+        <v>15941.587600000001</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="0"/>
+        <v>2380.4641000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J36">
+        <v>28.96</v>
+      </c>
+      <c r="K36">
+        <v>137.84</v>
+      </c>
+      <c r="L36">
+        <v>62.62</v>
+      </c>
+      <c r="M36">
+        <f>K36+L36</f>
+        <v>200.46</v>
+      </c>
+      <c r="N36">
+        <f>K36^2</f>
+        <v>18999.865600000001</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="0"/>
+        <v>3921.2643999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J37">
+        <v>27.86</v>
+      </c>
+      <c r="K37">
+        <v>114.24</v>
+      </c>
+      <c r="L37">
+        <v>19.309999999999999</v>
+      </c>
+      <c r="M37">
+        <f>K37+L37</f>
+        <v>133.54999999999998</v>
+      </c>
+      <c r="N37">
+        <f>K37^2</f>
+        <v>13050.777599999999</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="0"/>
+        <v>372.87609999999995</v>
+      </c>
+    </row>
+    <row r="38" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J38">
+        <v>28.75</v>
+      </c>
+      <c r="K38">
+        <v>31.73</v>
+      </c>
+      <c r="L38">
+        <v>67.33</v>
+      </c>
+      <c r="M38">
+        <f>K38+L38</f>
+        <v>99.06</v>
+      </c>
+      <c r="N38">
+        <f>K38^2</f>
+        <v>1006.7929</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="0"/>
+        <v>4533.3288999999995</v>
+      </c>
+    </row>
+    <row r="39" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J39">
+        <v>28.98</v>
+      </c>
+      <c r="K39">
+        <v>92.04</v>
+      </c>
+      <c r="L39">
+        <v>38.6</v>
+      </c>
+      <c r="M39">
+        <f>K39+L39</f>
+        <v>130.64000000000001</v>
+      </c>
+      <c r="N39">
+        <f>K39^2</f>
+        <v>8471.361600000002</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="0"/>
+        <v>1489.96</v>
+      </c>
+    </row>
+    <row r="40" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J40">
+        <v>62.94</v>
+      </c>
+      <c r="K40">
+        <v>59.06</v>
+      </c>
+      <c r="L40">
+        <v>18.350000000000001</v>
+      </c>
+      <c r="M40">
+        <f>K40+L40</f>
+        <v>77.41</v>
+      </c>
+      <c r="N40">
+        <f>K40^2</f>
+        <v>3488.0836000000004</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="0"/>
+        <v>336.72250000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J41">
+        <v>78.36</v>
+      </c>
+      <c r="K41">
+        <v>50.48</v>
+      </c>
+      <c r="L41">
+        <v>56.42</v>
+      </c>
+      <c r="M41">
+        <f>K41+L41</f>
+        <v>106.9</v>
+      </c>
+      <c r="N41">
+        <f>K41^2</f>
+        <v>2548.2303999999995</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="0"/>
+        <v>3183.2164000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J42">
+        <v>97.42</v>
+      </c>
+      <c r="K42">
+        <v>61.33</v>
+      </c>
+      <c r="L42">
+        <v>71.72</v>
+      </c>
+      <c r="M42">
+        <f>K42+L42</f>
+        <v>133.05000000000001</v>
+      </c>
+      <c r="N42">
+        <f>K42^2</f>
+        <v>3761.3688999999999</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="0"/>
+        <v>5143.7583999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J43">
+        <v>38.83</v>
+      </c>
+      <c r="K43">
+        <v>50.49</v>
+      </c>
+      <c r="L43">
+        <v>104.96</v>
+      </c>
+      <c r="M43">
+        <f>K43+L43</f>
+        <v>155.44999999999999</v>
+      </c>
+      <c r="N43">
+        <f>K43^2</f>
+        <v>2549.2401</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="0"/>
+        <v>11016.601599999998</v>
+      </c>
+    </row>
+    <row r="44" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J44">
+        <v>55.97</v>
+      </c>
+      <c r="K44">
+        <v>45.31</v>
+      </c>
+      <c r="L44">
+        <v>93.04</v>
+      </c>
+      <c r="M44">
+        <f>K44+L44</f>
+        <v>138.35000000000002</v>
+      </c>
+      <c r="N44">
+        <f>K44^2</f>
+        <v>2052.9961000000003</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="0"/>
+        <v>8656.4416000000019</v>
+      </c>
+    </row>
+    <row r="45" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J45">
+        <v>35.409999999999997</v>
+      </c>
+      <c r="K45">
+        <v>161.69</v>
+      </c>
+      <c r="L45">
+        <v>40.92</v>
+      </c>
+      <c r="M45">
+        <f>K45+L45</f>
+        <v>202.61</v>
+      </c>
+      <c r="N45">
+        <f>K45^2</f>
+        <v>26143.6561</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="0"/>
+        <v>1674.4464</v>
+      </c>
+    </row>
+    <row r="46" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J46">
+        <v>24.56</v>
+      </c>
+      <c r="K46">
+        <v>154.59</v>
+      </c>
+      <c r="L46">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="M46">
+        <f>K46+L46</f>
+        <v>195.36</v>
+      </c>
+      <c r="N46">
+        <f>K46^2</f>
+        <v>23898.0681</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="0"/>
+        <v>1662.1929000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J47">
+        <v>47.03</v>
+      </c>
+      <c r="K47">
+        <v>153.97999999999999</v>
+      </c>
+      <c r="L47">
+        <v>76.25</v>
+      </c>
+      <c r="M47">
+        <f>K47+L47</f>
+        <v>230.23</v>
+      </c>
+      <c r="N47">
+        <f>K47^2</f>
+        <v>23709.840399999997</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="0"/>
+        <v>5814.0625</v>
+      </c>
+    </row>
+    <row r="48" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J48">
+        <v>49.17</v>
+      </c>
+      <c r="K48">
+        <v>86.87</v>
+      </c>
+      <c r="L48">
+        <v>69.28</v>
+      </c>
+      <c r="M48">
+        <f>K48+L48</f>
+        <v>156.15</v>
+      </c>
+      <c r="N48">
+        <f>K48^2</f>
+        <v>7546.3969000000006</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="0"/>
+        <v>4799.7183999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J49">
+        <v>59.9</v>
+      </c>
+      <c r="K49">
+        <v>80.959999999999994</v>
+      </c>
+      <c r="L49">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="M49">
+        <f>K49+L49</f>
+        <v>146.56</v>
+      </c>
+      <c r="N49">
+        <f>K49^2</f>
+        <v>6554.5215999999991</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="0"/>
+        <v>4303.3599999999997</v>
+      </c>
+    </row>
+    <row r="50" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J50">
+        <v>149.55000000000001</v>
+      </c>
+      <c r="K50">
+        <v>56.52</v>
+      </c>
+      <c r="L50">
+        <v>24.73</v>
+      </c>
+      <c r="M50">
+        <f>K50+L50</f>
+        <v>81.25</v>
+      </c>
+      <c r="N50">
+        <f>K50^2</f>
+        <v>3194.5104000000006</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="0"/>
+        <v>611.5729</v>
+      </c>
+    </row>
+    <row r="51" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J51">
+        <v>256.73</v>
+      </c>
+      <c r="K51">
+        <v>34.909999999999997</v>
+      </c>
+      <c r="L51">
+        <v>131.6</v>
+      </c>
+      <c r="M51">
+        <f>K51+L51</f>
+        <v>166.51</v>
+      </c>
+      <c r="N51">
+        <f>K51^2</f>
+        <v>1218.7080999999998</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="0"/>
+        <v>17318.559999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J52">
+        <v>109.27</v>
+      </c>
+      <c r="K52">
+        <v>38.130000000000003</v>
+      </c>
+      <c r="L52">
+        <v>148.09</v>
+      </c>
+      <c r="M52">
+        <f>K52+L52</f>
+        <v>186.22</v>
+      </c>
+      <c r="N52">
+        <f>K52^2</f>
+        <v>1453.8969000000002</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="0"/>
+        <v>21930.648100000002</v>
+      </c>
+    </row>
+    <row r="53" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J53">
+        <v>95.84</v>
+      </c>
+      <c r="K53">
+        <v>66.58</v>
+      </c>
+      <c r="L53">
+        <v>82.8</v>
+      </c>
+      <c r="M53">
+        <f>K53+L53</f>
+        <v>149.38</v>
+      </c>
+      <c r="N53">
+        <f>K53^2</f>
+        <v>4432.8963999999996</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="0"/>
+        <v>6855.8399999999992</v>
+      </c>
+    </row>
+    <row r="54" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J54">
+        <v>87.91</v>
+      </c>
+      <c r="K54">
+        <v>94.23</v>
+      </c>
+      <c r="L54">
+        <v>33.1</v>
+      </c>
+      <c r="M54">
+        <f>K54+L54</f>
+        <v>127.33000000000001</v>
+      </c>
+      <c r="N54">
+        <f>K54^2</f>
+        <v>8879.2929000000004</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="0"/>
+        <v>1095.6100000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J55">
+        <v>81.290000000000006</v>
+      </c>
+      <c r="K55">
+        <v>178.7</v>
+      </c>
+      <c r="L55">
+        <v>19.760000000000002</v>
+      </c>
+      <c r="M55">
+        <f>K55+L55</f>
+        <v>198.45999999999998</v>
+      </c>
+      <c r="N55">
+        <f>K55^2</f>
+        <v>31933.689999999995</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="0"/>
+        <v>390.45760000000007</v>
+      </c>
+    </row>
+    <row r="56" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J56">
+        <v>239.16</v>
+      </c>
+      <c r="K56">
+        <v>218.14</v>
+      </c>
+      <c r="L56">
+        <v>90.98</v>
+      </c>
+      <c r="M56">
+        <f>K56+L56</f>
+        <v>309.12</v>
+      </c>
+      <c r="N56">
+        <f>K56^2</f>
+        <v>47585.059599999993</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="0"/>
+        <v>8277.3604000000014</v>
+      </c>
+    </row>
+    <row r="57" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J57">
+        <v>266.58999999999997</v>
+      </c>
+      <c r="K57">
+        <v>176.8</v>
+      </c>
+      <c r="L57">
+        <v>107.13</v>
+      </c>
+      <c r="M57">
+        <f>K57+L57</f>
+        <v>283.93</v>
+      </c>
+      <c r="N57">
+        <f>K57^2</f>
+        <v>31258.240000000005</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="0"/>
+        <v>11476.836899999998</v>
+      </c>
+    </row>
+    <row r="58" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J58">
+        <v>138.85</v>
+      </c>
+      <c r="K58">
+        <v>50.05</v>
+      </c>
+      <c r="L58">
+        <v>178.57</v>
+      </c>
+      <c r="M58">
+        <f>K58+L58</f>
+        <v>228.62</v>
+      </c>
+      <c r="N58">
+        <f>K58^2</f>
+        <v>2505.0024999999996</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="0"/>
+        <v>31887.244899999998</v>
+      </c>
+    </row>
+    <row r="59" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J59">
+        <v>139.15</v>
+      </c>
+      <c r="K59">
+        <v>40.43</v>
+      </c>
+      <c r="L59">
+        <v>28.02</v>
+      </c>
+      <c r="M59">
+        <f>K59+L59</f>
+        <v>68.45</v>
+      </c>
+      <c r="N59">
+        <f>K59^2</f>
+        <v>1634.5849000000001</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="0"/>
+        <v>785.12040000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J60">
+        <v>201.42</v>
+      </c>
+      <c r="K60">
+        <v>18.66</v>
+      </c>
+      <c r="L60">
+        <v>198.53</v>
+      </c>
+      <c r="M60">
+        <f>K60+L60</f>
+        <v>217.19</v>
+      </c>
+      <c r="N60">
+        <f>K60^2</f>
+        <v>348.19560000000001</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="0"/>
+        <v>39414.160900000003</v>
+      </c>
+    </row>
+    <row r="61" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J61">
+        <v>123.97</v>
+      </c>
+      <c r="K61">
+        <v>201.53</v>
+      </c>
+      <c r="L61">
+        <v>99.78</v>
+      </c>
+      <c r="M61">
+        <f>K61+L61</f>
+        <v>301.31</v>
+      </c>
+      <c r="N61">
+        <f>K61^2</f>
+        <v>40614.340900000003</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="0"/>
+        <v>9956.0483999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J62">
+        <v>358.79</v>
+      </c>
+      <c r="K62">
+        <v>563.69000000000005</v>
+      </c>
+      <c r="L62">
+        <v>405.17</v>
+      </c>
+      <c r="M62">
+        <f>K62+L62</f>
+        <v>968.86000000000013</v>
+      </c>
+      <c r="N62">
+        <f>K62^2</f>
+        <v>317746.41610000009</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="0"/>
+        <v>164162.72890000002</v>
+      </c>
+    </row>
+    <row r="63" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J63">
+        <v>875.73</v>
+      </c>
+      <c r="K63">
+        <v>724.93</v>
+      </c>
+      <c r="L63">
+        <v>745.69</v>
+      </c>
+      <c r="M63">
+        <f>K63+L63</f>
+        <v>1470.62</v>
+      </c>
+      <c r="N63">
+        <f>K63^2</f>
+        <v>525523.50489999994</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="0"/>
+        <v>556053.57610000006</v>
+      </c>
+    </row>
+    <row r="64" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J64">
+        <v>1240.48</v>
+      </c>
+      <c r="K64">
+        <v>1432.46</v>
+      </c>
+      <c r="L64">
+        <v>1693.71</v>
+      </c>
+      <c r="M64">
+        <f>K64+L64</f>
+        <v>3126.17</v>
+      </c>
+      <c r="N64">
+        <f>K64^2</f>
+        <v>2051941.6516000002</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="0"/>
+        <v>2868653.5641000001</v>
+      </c>
+    </row>
+    <row r="65" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="J65">
+        <v>1334.54</v>
+      </c>
+      <c r="K65">
+        <v>4620.0200000000004</v>
+      </c>
+      <c r="L65">
+        <v>5316</v>
+      </c>
+      <c r="M65">
+        <f>K65+L65</f>
+        <v>9936.02</v>
+      </c>
+      <c r="N65">
+        <f>K65^2</f>
+        <v>21344584.800400004</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="0"/>
+        <v>28259856</v>
+      </c>
+    </row>
+    <row r="66" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="L66" t="s">
+        <v>7</v>
+      </c>
+      <c r="M66">
+        <f>SUM(M2:M65)</f>
+        <v>55764.070000000022</v>
+      </c>
+      <c r="N66">
+        <f t="shared" ref="N66:O66" si="1">SUM(N2:N65)</f>
+        <v>99397748.581399962</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="1"/>
+        <v>134097028.7013</v>
+      </c>
+    </row>
+    <row r="68" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="K68" t="s">
+        <v>8</v>
+      </c>
+      <c r="M68">
+        <f>M66/SQRT(N66*O66)</f>
+        <v>4.8301054521103498E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="10:15" x14ac:dyDescent="0.35">
+      <c r="M72">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="N72">
+        <f>M72*1000</f>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>